<commit_message>
add venv and bug fix
</commit_message>
<xml_diff>
--- a/ol.xlsx
+++ b/ol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t xml:space="preserve">فلافل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">برنج ایرانی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">۱۳۰</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -218,12 +224,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -290,6 +296,17 @@
       </c>
       <c r="C5" s="0" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -323,17 +340,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>